<commit_message>
Output updated in Threshold_Results
</commit_message>
<xml_diff>
--- a/Threshold_Results/Threshold_Results.xlsx
+++ b/Threshold_Results/Threshold_Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30520" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="5860" yWindow="0" windowWidth="32120" windowHeight="14100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Welfare_Gain_Pop(bench)</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>wage_exp</t>
+  </si>
+  <si>
+    <t>Share_Above_Threshold</t>
   </si>
 </sst>
 </file>
@@ -116,7 +119,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -277,7 +280,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="131">
+  <cellStyleXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -409,28 +412,87 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="131">
+  <cellStyles count="189">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -496,6 +558,35 @@
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -561,6 +652,35 @@
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -890,23 +1010,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="16" width="8.5" customWidth="1"/>
+    <col min="4" max="20" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:16">
-      <c r="P1" s="3"/>
+    <row r="1" spans="3:24">
+      <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="3:16">
+    <row r="2" spans="3:24">
       <c r="C2" s="13" t="s">
         <v>13</v>
       </c>
@@ -941,14 +1061,37 @@
         <v>2.25</v>
       </c>
       <c r="N2" s="12">
+        <v>2.3999999999999901</v>
+      </c>
+      <c r="O2" s="12">
         <v>2.5</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="5">
+      <c r="P2" s="12">
+        <v>2.6</v>
+      </c>
+      <c r="Q2" s="12">
+        <v>2.7</v>
+      </c>
+      <c r="R2" s="12">
+        <v>2.71</v>
+      </c>
+      <c r="S2" s="12">
+        <v>2.8999999999999901</v>
+      </c>
+      <c r="T2" s="12">
         <v>3</v>
       </c>
+      <c r="U2" s="12">
+        <v>3.1</v>
+      </c>
+      <c r="V2" s="12">
+        <v>3.2</v>
+      </c>
+      <c r="W2" s="14">
+        <v>3.2999999999999901</v>
+      </c>
     </row>
-    <row r="3" spans="3:16">
+    <row r="3" spans="3:24">
       <c r="C3" s="10" t="s">
         <v>14</v>
       </c>
@@ -983,14 +1126,37 @@
         <v>0.62028891396452901</v>
       </c>
       <c r="N3" s="2">
+        <v>0.66164150822883105</v>
+      </c>
+      <c r="O3" s="2">
         <v>0.68920990440503305</v>
       </c>
-      <c r="O3" s="2"/>
-      <c r="P3" s="5">
+      <c r="P3" s="2">
+        <v>0.71677830058123404</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0.74434669675743503</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0.747103536375055</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0.79948348910983802</v>
+      </c>
+      <c r="T3" s="2">
         <v>0.82705188528603901</v>
       </c>
+      <c r="U3" s="2">
+        <v>0.854620281462241</v>
+      </c>
+      <c r="V3" s="2">
+        <v>0.882188677638442</v>
+      </c>
+      <c r="W3" s="5">
+        <v>0.90975707381464299</v>
+      </c>
     </row>
-    <row r="4" spans="3:16">
+    <row r="4" spans="3:24">
       <c r="C4" s="10" t="s">
         <v>15</v>
       </c>
@@ -1025,14 +1191,37 @@
         <v>2.8654108781147301</v>
       </c>
       <c r="N4" s="2">
+        <v>3.05643826998904</v>
+      </c>
+      <c r="O4" s="2">
         <v>3.1837898645719198</v>
       </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="5">
+      <c r="P4" s="2">
+        <v>3.3111414591548001</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>3.4384930537376701</v>
+      </c>
+      <c r="R4" s="2">
+        <v>3.45122821319596</v>
+      </c>
+      <c r="S4" s="2">
+        <v>3.6931962429034302</v>
+      </c>
+      <c r="T4" s="2">
         <v>3.82054783748631</v>
       </c>
+      <c r="U4" s="2">
+        <v>3.94789943206918</v>
+      </c>
+      <c r="V4" s="2">
+        <v>4.0752510266520598</v>
+      </c>
+      <c r="W4" s="5">
+        <v>4.2026026212349397</v>
+      </c>
     </row>
-    <row r="5" spans="3:16">
+    <row r="5" spans="3:24">
       <c r="C5" s="10" t="s">
         <v>16</v>
       </c>
@@ -1069,12 +1258,35 @@
       <c r="N5" s="1">
         <v>0</v>
       </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="6">
+      <c r="O5" s="1">
         <v>0</v>
       </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
+        <v>0</v>
+      </c>
+      <c r="V5" s="1">
+        <v>0</v>
+      </c>
+      <c r="W5" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="3:16">
+    <row r="6" spans="3:24">
       <c r="C6" s="10" t="s">
         <v>17</v>
       </c>
@@ -1106,17 +1318,41 @@
         <v>2.34046377468713E-2</v>
       </c>
       <c r="M6" s="2">
-        <v>2.4995455398512799E-2</v>
+        <v>2.4057250858187801E-2</v>
       </c>
       <c r="N6" s="2">
-        <v>2.2485674335389502E-2</v>
-      </c>
-      <c r="O6" s="2"/>
-      <c r="P6" s="5">
-        <v>2.8233231735055E-2</v>
-      </c>
+        <v>2.34479142877035E-2</v>
+      </c>
+      <c r="O6" s="2">
+        <v>2.3010639400186599E-2</v>
+      </c>
+      <c r="P6" s="2">
+        <v>2.318833827732E-2</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>2.4900693610104101E-2</v>
+      </c>
+      <c r="R6" s="2">
+        <v>2.48113227152124E-2</v>
+      </c>
+      <c r="S6" s="2">
+        <v>2.9987753695654699E-2</v>
+      </c>
+      <c r="T6" s="2">
+        <v>2.8167066107881899E-2</v>
+      </c>
+      <c r="U6" s="2">
+        <v>2.6948411241147999E-2</v>
+      </c>
+      <c r="V6" s="2">
+        <v>2.58291980071092E-2</v>
+      </c>
+      <c r="W6" s="5">
+        <v>2.5172367447682299E-2</v>
+      </c>
+      <c r="X6" s="18"/>
     </row>
-    <row r="7" spans="3:16">
+    <row r="7" spans="3:24">
       <c r="C7" s="10" t="s">
         <v>0</v>
       </c>
@@ -1148,17 +1384,40 @@
         <v>1.02202648232615</v>
       </c>
       <c r="M7" s="2">
-        <v>0.91988317030746303</v>
+        <v>1.08300543945159</v>
       </c>
       <c r="N7" s="2">
-        <v>1.3183638391122201</v>
-      </c>
-      <c r="O7" s="2"/>
-      <c r="P7" s="5">
-        <v>0.748932034723647</v>
+        <v>1.1660027599585601</v>
+      </c>
+      <c r="O7" s="2">
+        <v>1.22262862059735</v>
+      </c>
+      <c r="P7" s="2">
+        <v>1.2043070021629001</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>1.0199830574669599</v>
+      </c>
+      <c r="R7" s="2">
+        <v>1.0339221939508501</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0.50938275050976001</v>
+      </c>
+      <c r="T7" s="2">
+        <v>0.75891207125746396</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0.92559997388427795</v>
+      </c>
+      <c r="V7" s="2">
+        <v>1.08351357411659</v>
+      </c>
+      <c r="W7" s="5">
+        <v>1.1741706331275501</v>
       </c>
     </row>
-    <row r="8" spans="3:16">
+    <row r="8" spans="3:24">
       <c r="C8" s="10" t="s">
         <v>1</v>
       </c>
@@ -1190,17 +1449,40 @@
         <v>1.1293247605229599</v>
       </c>
       <c r="M8" s="2">
-        <v>1.06981109933202</v>
+        <v>1.21442723536232</v>
       </c>
       <c r="N8" s="2">
-        <v>1.38891890765493</v>
-      </c>
-      <c r="O8" s="2"/>
-      <c r="P8" s="5">
-        <v>0.96637119175474095</v>
+        <v>1.26881226178683</v>
+      </c>
+      <c r="O8" s="2">
+        <v>1.3027888339331199</v>
+      </c>
+      <c r="P8" s="2">
+        <v>1.27821700703257</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>1.1254416989196701</v>
+      </c>
+      <c r="R8" s="2">
+        <v>1.1366809267806599</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0.78535833021317203</v>
+      </c>
+      <c r="T8" s="2">
+        <v>0.97472450876405703</v>
+      </c>
+      <c r="U8" s="2">
+        <v>1.0982862363683901</v>
+      </c>
+      <c r="V8" s="2">
+        <v>1.21561959462682</v>
+      </c>
+      <c r="W8" s="5">
+        <v>1.2776294140572899</v>
       </c>
     </row>
-    <row r="9" spans="3:16">
+    <row r="9" spans="3:24">
       <c r="C9" s="10" t="s">
         <v>2</v>
       </c>
@@ -1232,17 +1514,40 @@
         <v>1.9932467656578501</v>
       </c>
       <c r="M9" s="2">
-        <v>1.78977958739993</v>
+        <v>2.07102995002277</v>
       </c>
       <c r="N9" s="2">
-        <v>2.4960583455598901</v>
-      </c>
-      <c r="O9" s="2"/>
-      <c r="P9" s="5">
-        <v>1.3575845152618999</v>
+        <v>2.2254911424231798</v>
+      </c>
+      <c r="O9" s="2">
+        <v>2.330913073234</v>
+      </c>
+      <c r="P9" s="2">
+        <v>2.2833428346972502</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>1.8892204599056901</v>
+      </c>
+      <c r="R9" s="2">
+        <v>1.91345949719007</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0.92809594651778404</v>
+      </c>
+      <c r="T9" s="2">
+        <v>1.37496897980774</v>
+      </c>
+      <c r="U9" s="2">
+        <v>1.67343377806884</v>
+      </c>
+      <c r="V9" s="2">
+        <v>1.96125627857815</v>
+      </c>
+      <c r="W9" s="5">
+        <v>2.1238905986347598</v>
       </c>
     </row>
-    <row r="10" spans="3:16">
+    <row r="10" spans="3:24">
       <c r="C10" s="10" t="s">
         <v>3</v>
       </c>
@@ -1274,17 +1579,40 @@
         <v>2.0610552344931201</v>
       </c>
       <c r="M10" s="2">
-        <v>1.89450751845807</v>
+        <v>2.16311186982588</v>
       </c>
       <c r="N10" s="2">
-        <v>2.5500954367034399</v>
-      </c>
-      <c r="O10" s="2"/>
-      <c r="P10" s="5">
-        <v>1.5205878421314001</v>
+        <v>2.3001726745956899</v>
+      </c>
+      <c r="O10" s="2">
+        <v>2.3931339569552299</v>
+      </c>
+      <c r="P10" s="2">
+        <v>2.3430284562510901</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>1.97086768040066</v>
+      </c>
+      <c r="R10" s="2">
+        <v>1.9929899097439101</v>
+      </c>
+      <c r="S10" s="2">
+        <v>1.1296878063176801</v>
+      </c>
+      <c r="T10" s="2">
+        <v>1.53706613172033</v>
+      </c>
+      <c r="U10" s="2">
+        <v>1.8073710970485699</v>
+      </c>
+      <c r="V10" s="2">
+        <v>2.0699887396671399</v>
+      </c>
+      <c r="W10" s="5">
+        <v>2.2149818094293998</v>
       </c>
     </row>
-    <row r="11" spans="3:16">
+    <row r="11" spans="3:24">
       <c r="C11" s="10" t="s">
         <v>18</v>
       </c>
@@ -1316,17 +1644,40 @@
         <v>2.7584754841220902</v>
       </c>
       <c r="M11" s="2">
-        <v>2.1214298177323299</v>
+        <v>2.5048682999011298</v>
       </c>
       <c r="N11" s="2">
-        <v>3.1734068110865499</v>
-      </c>
-      <c r="O11" s="2"/>
-      <c r="P11" s="5">
-        <v>0.99211223991377795</v>
+        <v>2.7779709622625099</v>
+      </c>
+      <c r="O11" s="2">
+        <v>2.96660287850758</v>
+      </c>
+      <c r="P11" s="2">
+        <v>2.9004209389471498</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>2.20351338384532</v>
+      </c>
+      <c r="R11" s="2">
+        <v>2.2394373649551702</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0.33878568991005897</v>
+      </c>
+      <c r="T11" s="2">
+        <v>1.01247827066859</v>
+      </c>
+      <c r="U11" s="2">
+        <v>1.47657950518074</v>
+      </c>
+      <c r="V11" s="2">
+        <v>1.9178861640740801</v>
+      </c>
+      <c r="W11" s="5">
+        <v>2.1777692649262299</v>
       </c>
     </row>
-    <row r="12" spans="3:16">
+    <row r="12" spans="3:24">
       <c r="C12" s="10" t="s">
         <v>4</v>
       </c>
@@ -1358,17 +1709,40 @@
         <v>3.0390796197143599</v>
       </c>
       <c r="M12" s="2">
-        <v>3.0121420008313899</v>
+        <v>3.0395980878806701</v>
       </c>
       <c r="N12" s="2">
-        <v>3.0918426470638001</v>
-      </c>
-      <c r="O12" s="2"/>
-      <c r="P12" s="5">
-        <v>2.9927303368992302</v>
+        <v>3.0617731281740999</v>
+      </c>
+      <c r="O12" s="2">
+        <v>3.0780175983129601</v>
+      </c>
+      <c r="P12" s="2">
+        <v>3.0785863231738602</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>3.0468287027375101</v>
+      </c>
+      <c r="R12" s="2">
+        <v>3.0493091455272898</v>
+      </c>
+      <c r="S12" s="2">
+        <v>2.9526572087755998</v>
+      </c>
+      <c r="T12" s="2">
+        <v>2.9941371128259102</v>
+      </c>
+      <c r="U12" s="2">
+        <v>3.0253284284605702</v>
+      </c>
+      <c r="V12" s="2">
+        <v>3.0547790426824002</v>
+      </c>
+      <c r="W12" s="5">
+        <v>3.0731488198646102</v>
       </c>
     </row>
-    <row r="13" spans="3:16">
+    <row r="13" spans="3:24">
       <c r="C13" s="10" t="s">
         <v>19</v>
       </c>
@@ -1400,17 +1774,40 @@
         <v>0.404098122893223</v>
       </c>
       <c r="M13" s="2">
-        <v>0.39356771992593398</v>
+        <v>0.39646835698079502</v>
       </c>
       <c r="N13" s="2">
-        <v>0.39335762326753199</v>
-      </c>
-      <c r="O13" s="2"/>
-      <c r="P13" s="5">
-        <v>0.37372440945461599</v>
+        <v>0.39456102934855303</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0.39305064111320598</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0.39135678562870502</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>0.38700053316143601</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0.386945694969898</v>
+      </c>
+      <c r="S13" s="2">
+        <v>0.37281455407932601</v>
+      </c>
+      <c r="T13" s="2">
+        <v>0.37375218895909401</v>
+      </c>
+      <c r="U13" s="2">
+        <v>0.37415472130435801</v>
+      </c>
+      <c r="V13" s="2">
+        <v>0.374308430265409</v>
+      </c>
+      <c r="W13" s="5">
+        <v>0.37380504567107797</v>
       </c>
     </row>
-    <row r="14" spans="3:16">
+    <row r="14" spans="3:24">
       <c r="C14" s="10" t="s">
         <v>20</v>
       </c>
@@ -1442,17 +1839,40 @@
         <v>0.73857074220492902</v>
       </c>
       <c r="M14" s="2">
-        <v>0.72490684945127903</v>
+        <v>0.72765813234278198</v>
       </c>
       <c r="N14" s="2">
-        <v>0.72599976232738495</v>
-      </c>
-      <c r="O14" s="2"/>
-      <c r="P14" s="5">
-        <v>0.69118837298924596</v>
+        <v>0.72609821300695099</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0.72474760012175299</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0.72214244517957105</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>0.71314261618886898</v>
+      </c>
+      <c r="R14" s="2">
+        <v>0.71318530048182704</v>
+      </c>
+      <c r="S14" s="2">
+        <v>0.68721170250473695</v>
+      </c>
+      <c r="T14" s="2">
+        <v>0.69135331362953401</v>
+      </c>
+      <c r="U14" s="2">
+        <v>0.69382485413646799</v>
+      </c>
+      <c r="V14" s="2">
+        <v>0.69575709510928396</v>
+      </c>
+      <c r="W14" s="5">
+        <v>0.69620780827763795</v>
       </c>
     </row>
-    <row r="15" spans="3:16">
+    <row r="15" spans="3:24">
       <c r="C15" s="10" t="s">
         <v>21</v>
       </c>
@@ -1484,17 +1904,40 @@
         <v>0.800929254486065</v>
       </c>
       <c r="M15" s="2">
-        <v>0.80561504268491102</v>
+        <v>0.80552216170251001</v>
       </c>
       <c r="N15" s="2">
-        <v>0.80634062253227601</v>
-      </c>
-      <c r="O15" s="2"/>
-      <c r="P15" s="5">
-        <v>0.81406322341426496</v>
+        <v>0.80608798178173902</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0.80649032033537005</v>
+      </c>
+      <c r="P15" s="2">
+        <v>0.806625904102103</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>0.80736170747582103</v>
+      </c>
+      <c r="R15" s="2">
+        <v>0.80741077034514996</v>
+      </c>
+      <c r="S15" s="2">
+        <v>0.81447971716795198</v>
+      </c>
+      <c r="T15" s="2">
+        <v>0.81403743338873202</v>
+      </c>
+      <c r="U15" s="2">
+        <v>0.81397320688796304</v>
+      </c>
+      <c r="V15" s="2">
+        <v>0.81388981787098602</v>
+      </c>
+      <c r="W15" s="5">
+        <v>0.81403926578683605</v>
       </c>
     </row>
-    <row r="16" spans="3:16">
+    <row r="16" spans="3:24">
       <c r="C16" s="10" t="s">
         <v>22</v>
       </c>
@@ -1526,17 +1969,40 @@
         <v>0.40404640068583297</v>
       </c>
       <c r="M16" s="2">
-        <v>0.402784863168824</v>
+        <v>0.40286036825098698</v>
       </c>
       <c r="N16" s="2">
-        <v>0.40271153138107202</v>
-      </c>
-      <c r="O16" s="2"/>
-      <c r="P16" s="5">
-        <v>0.40050998110281799</v>
+        <v>0.40276707122212102</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0.40273366878711098</v>
+      </c>
+      <c r="P16" s="2">
+        <v>0.40264320549069099</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>0.40221175173773799</v>
+      </c>
+      <c r="R16" s="2">
+        <v>0.40220931468120502</v>
+      </c>
+      <c r="S16" s="2">
+        <v>0.40038702323415598</v>
+      </c>
+      <c r="T16" s="2">
+        <v>0.40049947018520998</v>
+      </c>
+      <c r="U16" s="2">
+        <v>0.40055682328105202</v>
+      </c>
+      <c r="V16" s="2">
+        <v>0.40062561400485303</v>
+      </c>
+      <c r="W16" s="5">
+        <v>0.400644220628043</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:24">
       <c r="B17" s="2"/>
       <c r="C17" s="10" t="s">
         <v>5</v>
@@ -1569,354 +2035,588 @@
         <v>6.46931021800453E-3</v>
       </c>
       <c r="M17" s="2">
-        <v>3.2784271300385298E-3</v>
+        <v>5.1071695181510298E-3</v>
       </c>
       <c r="N17" s="2">
-        <v>1.1585656071506001E-2</v>
-      </c>
-      <c r="O17" s="2"/>
-      <c r="P17" s="5">
-        <v>1.74209543897771E-3</v>
-      </c>
+        <v>7.0966979553278202E-3</v>
+      </c>
+      <c r="O17" s="2">
+        <v>9.1682050814899992E-3</v>
+      </c>
+      <c r="P17" s="2">
+        <v>9.0116577354749493E-3</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>4.4709401367571096E-3</v>
+      </c>
+      <c r="R17" s="2">
+        <v>4.7052368364675799E-3</v>
+      </c>
+      <c r="S17" s="2">
+        <v>4.0472533393222897E-3</v>
+      </c>
+      <c r="T17" s="2">
+        <v>1.7185816247539301E-3</v>
+      </c>
+      <c r="U17" s="2">
+        <v>2.2652701822673499E-3</v>
+      </c>
+      <c r="V17" s="2">
+        <v>4.5739906775750603E-3</v>
+      </c>
+      <c r="W17" s="5">
+        <v>6.8812715169669697E-3</v>
+      </c>
+      <c r="X17" s="18"/>
     </row>
-    <row r="18" spans="1:16">
-      <c r="A18" s="16" t="s">
+    <row r="18" spans="1:24">
+      <c r="B18" s="2"/>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2">
+        <v>0.26124077464275702</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0.26833021178133099</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0.27398371885989198</v>
+      </c>
+      <c r="P18" s="2">
+        <v>0.27142219872036999</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>0.25145415339782601</v>
+      </c>
+      <c r="R18" s="2">
+        <v>0.25198114641110397</v>
+      </c>
+      <c r="S18" s="2">
+        <v>0.217501956930787</v>
+      </c>
+      <c r="T18" s="2">
+        <v>0.22354916889552801</v>
+      </c>
+      <c r="U18" s="2">
+        <v>0.228569345971396</v>
+      </c>
+      <c r="V18" s="2">
+        <v>0.23349135428363599</v>
+      </c>
+      <c r="W18" s="5">
+        <v>0.237206078062977</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24">
+      <c r="A19" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B19" s="12">
         <v>0.30417415268987902</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C19" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D19" s="12">
         <v>0.30407904083248399</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E19" s="12">
         <v>0.30444046050060902</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F19" s="12">
         <v>0.304448201690313</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G19" s="12">
         <v>0.30435464741558899</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H19" s="12">
         <v>0.304273607737365</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I19" s="12">
         <v>0.30444526778318698</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J19" s="12">
         <v>0.30400698703752999</v>
       </c>
-      <c r="K18" s="12">
+      <c r="K19" s="12">
         <v>0.30444556015124102</v>
       </c>
-      <c r="L18" s="12">
+      <c r="L19" s="12">
         <v>0.30447659970902102</v>
       </c>
-      <c r="M18" s="12">
-        <v>0.30445191118794901</v>
-      </c>
-      <c r="N18" s="12">
-        <v>0.30402161857613302</v>
-      </c>
-      <c r="O18" s="12"/>
-      <c r="P18" s="14">
-        <v>0.30412549111529902</v>
+      <c r="M19" s="12">
+        <v>0.30406172967433998</v>
+      </c>
+      <c r="N19" s="12">
+        <v>0.30430791571078503</v>
+      </c>
+      <c r="O19" s="12">
+        <v>0.30446027608103998</v>
+      </c>
+      <c r="P19" s="12">
+        <v>0.30445569226714803</v>
+      </c>
+      <c r="Q19" s="12">
+        <v>0.30409746147066502</v>
+      </c>
+      <c r="R19" s="12">
+        <v>0.30409006202178102</v>
+      </c>
+      <c r="S19" s="12">
+        <v>0.30413201979252102</v>
+      </c>
+      <c r="T19" s="12">
+        <v>0.30407563913759</v>
+      </c>
+      <c r="U19" s="12">
+        <v>0.30409383126553702</v>
+      </c>
+      <c r="V19" s="12">
+        <v>0.30409107990696499</v>
+      </c>
+      <c r="W19" s="14">
+        <v>0.30408412810455898</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
-      <c r="A19" s="8" t="s">
+    <row r="20" spans="1:24">
+      <c r="A20" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B20" s="15">
         <v>8.4907023270955602</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C20" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D20" s="15">
         <v>9.6071550742049698</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E20" s="15">
         <v>9.5696187225203992</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F20" s="15">
         <v>9.6021411467766793</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G20" s="15">
         <v>9.5726645774687409</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H20" s="15">
         <v>9.5595896805572007</v>
       </c>
-      <c r="I19" s="15">
+      <c r="I20" s="15">
         <v>9.44207547138077</v>
       </c>
-      <c r="J19" s="15">
+      <c r="J20" s="15">
         <v>9.3954546478243604</v>
       </c>
-      <c r="K19" s="15">
+      <c r="K20" s="15">
         <v>9.3521741092699795</v>
       </c>
-      <c r="L19" s="15">
+      <c r="L20" s="15">
         <v>9.20377061416864</v>
       </c>
-      <c r="M19" s="15">
-        <v>9.0554286157570303</v>
-      </c>
-      <c r="N19" s="15">
-        <v>9.3448119693713494</v>
-      </c>
-      <c r="O19" s="15"/>
-      <c r="P19" s="5">
-        <v>8.80182743650278</v>
+      <c r="M20" s="15">
+        <v>9.1579311720199907</v>
+      </c>
+      <c r="N20" s="15">
+        <v>9.2330361654004793</v>
+      </c>
+      <c r="O20" s="15">
+        <v>9.2859668007345295</v>
+      </c>
+      <c r="P20" s="15">
+        <v>9.2721089813455499</v>
+      </c>
+      <c r="Q20" s="15">
+        <v>9.0975930827476894</v>
+      </c>
+      <c r="R20" s="15">
+        <v>9.1073797758124204</v>
+      </c>
+      <c r="S20" s="15">
+        <v>8.6315526584094293</v>
+      </c>
+      <c r="T20" s="15">
+        <v>8.8077572473754007</v>
+      </c>
+      <c r="U20" s="15">
+        <v>8.93052168301592</v>
+      </c>
+      <c r="V20" s="15">
+        <v>9.0495190411743405</v>
+      </c>
+      <c r="W20" s="5">
+        <v>9.1206603132552697</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
-      <c r="A20" s="8" t="s">
+    <row r="21" spans="1:24">
+      <c r="A21" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B21" s="15">
         <v>0.56606848946940602</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D21" s="15">
         <v>0.570202364536471</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E21" s="15">
         <v>0.56982514083142399</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F21" s="15">
         <v>0.56933745334098496</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G21" s="15">
         <v>0.56882534465068402</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H21" s="15">
         <v>0.56834397707043305</v>
       </c>
-      <c r="I20" s="15">
+      <c r="I21" s="15">
         <v>0.56795143305868001</v>
       </c>
-      <c r="J20" s="15">
+      <c r="J21" s="15">
         <v>0.56736002289600795</v>
       </c>
-      <c r="K20" s="15">
+      <c r="K21" s="15">
         <v>0.56704073055711501</v>
       </c>
-      <c r="L20" s="15">
+      <c r="L21" s="15">
         <v>0.56657517507708399</v>
       </c>
-      <c r="M20" s="15">
-        <v>0.56585124140444798</v>
-      </c>
-      <c r="N20" s="15">
-        <v>0.56573957280973697</v>
-      </c>
-      <c r="O20" s="15"/>
-      <c r="P20" s="5">
-        <v>0.56437814335756198</v>
+      <c r="M21" s="15">
+        <v>0.56587933291932202</v>
+      </c>
+      <c r="N21" s="15">
+        <v>0.56585013190469902</v>
+      </c>
+      <c r="O21" s="15">
+        <v>0.56580558209391996</v>
+      </c>
+      <c r="P21" s="15">
+        <v>0.56567882363506605</v>
+      </c>
+      <c r="Q21" s="15">
+        <v>0.56523544090940903</v>
+      </c>
+      <c r="R21" s="15">
+        <v>0.56523259590576802</v>
+      </c>
+      <c r="S21" s="15">
+        <v>0.56434144879480996</v>
+      </c>
+      <c r="T21" s="15">
+        <v>0.56436078470335005</v>
+      </c>
+      <c r="U21" s="15">
+        <v>0.56437436345380398</v>
+      </c>
+      <c r="V21" s="15">
+        <v>0.56435017135881504</v>
+      </c>
+      <c r="W21" s="5">
+        <v>0.56431865726974995</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
-      <c r="A21" s="8" t="s">
+    <row r="22" spans="1:24">
+      <c r="A22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B22" s="2">
         <v>1.38348230839374</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C22" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D22" s="2">
         <v>1.4480905640906301</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E22" s="2">
         <v>1.4455799161803</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F22" s="2">
         <v>1.4463693287064201</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G22" s="2">
         <v>1.44403169825758</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H22" s="2">
         <v>1.44256203589742</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I22" s="2">
         <v>1.4360209242695201</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J22" s="2">
         <v>1.4326767869102099</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K22" s="2">
         <v>1.4299560965270199</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L22" s="2">
         <v>1.42164532869795</v>
       </c>
-      <c r="M21" s="2">
-        <v>1.41283191460706</v>
-      </c>
-      <c r="N21" s="2">
-        <v>1.4273858301984901</v>
-      </c>
-      <c r="O21" s="2"/>
-      <c r="P21" s="5">
-        <v>1.3972080057123599</v>
+      <c r="M22" s="2">
+        <v>1.4181367181714399</v>
+      </c>
+      <c r="N22" s="2">
+        <v>1.4219150451889599</v>
+      </c>
+      <c r="O22" s="2">
+        <v>1.4245247343781999</v>
+      </c>
+      <c r="P22" s="2">
+        <v>1.42360911895303</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>1.4139675262223299</v>
+      </c>
+      <c r="R22" s="2">
+        <v>1.41446452814546</v>
+      </c>
+      <c r="S22" s="2">
+        <v>1.3881693484770199</v>
+      </c>
+      <c r="T22" s="2">
+        <v>1.3974897661447701</v>
+      </c>
+      <c r="U22" s="2">
+        <v>1.40391052461729</v>
+      </c>
+      <c r="V22" s="2">
+        <v>1.4100159241688399</v>
+      </c>
+      <c r="W22" s="5">
+        <v>1.4136113608916301</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
-      <c r="A22" s="8" t="s">
+    <row r="23" spans="1:24">
+      <c r="A23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B23" s="2">
         <v>1.2735159458287599</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C23" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D23" s="2">
         <v>1.33298880165277</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E23" s="2">
         <v>1.3306777130839</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F23" s="2">
         <v>1.3314043790005901</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G23" s="2">
         <v>1.3292525555663499</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H23" s="2">
         <v>1.3278997096070699</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I23" s="2">
         <v>1.3218785195195399</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J23" s="2">
         <v>1.31880019157398</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K23" s="2">
         <v>1.31629575579938</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L23" s="2">
         <v>1.30864557098084</v>
       </c>
-      <c r="M22" s="2">
-        <v>1.3005326928371499</v>
-      </c>
-      <c r="N22" s="2">
-        <v>1.3139297875939699</v>
-      </c>
-      <c r="O22" s="2"/>
-      <c r="P22" s="5">
-        <v>1.2861506534045899</v>
+      <c r="M23" s="2">
+        <v>1.30541584305002</v>
+      </c>
+      <c r="N23" s="2">
+        <v>1.3088938490036699</v>
+      </c>
+      <c r="O23" s="2">
+        <v>1.3112961065359701</v>
+      </c>
+      <c r="P23" s="2">
+        <v>1.31045326898241</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>1.3015780401405099</v>
+      </c>
+      <c r="R23" s="2">
+        <v>1.3020355377683199</v>
+      </c>
+      <c r="S23" s="2">
+        <v>1.2778304356119601</v>
+      </c>
+      <c r="T23" s="2">
+        <v>1.2864100180537801</v>
+      </c>
+      <c r="U23" s="2">
+        <v>1.2923204212800801</v>
+      </c>
+      <c r="V23" s="2">
+        <v>1.2979405319510899</v>
+      </c>
+      <c r="W23" s="5">
+        <v>1.3012501846809601</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
-      <c r="A23" s="8" t="s">
+    <row r="24" spans="1:24">
+      <c r="A24" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B24" s="2">
         <v>6.65944897877669E-2</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C24" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D24" s="2">
         <v>6.2369798745459802E-2</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E24" s="2">
         <v>6.2481417604323602E-2</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F24" s="2">
         <v>6.2324939635978197E-2</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G24" s="2">
         <v>6.23966263574934E-2</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H24" s="2">
         <v>6.2409846139746497E-2</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I24" s="2">
         <v>6.2822322395599303E-2</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J24" s="2">
         <v>6.2955857493994502E-2</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K24" s="2">
         <v>6.30979599967708E-2</v>
       </c>
-      <c r="L23" s="2">
+      <c r="L24" s="2">
         <v>6.3640853387662899E-2</v>
       </c>
-      <c r="M23" s="2">
-        <v>6.4178021783205003E-2</v>
-      </c>
-      <c r="N23" s="2">
-        <v>6.3029202278085603E-2</v>
-      </c>
-      <c r="O23" s="2"/>
-      <c r="P23" s="5">
-        <v>6.5111760866712706E-2</v>
-      </c>
+      <c r="M24" s="2">
+        <v>6.3769704430609295E-2</v>
+      </c>
+      <c r="N24" s="2">
+        <v>6.3471316493983895E-2</v>
+      </c>
+      <c r="O24" s="2">
+        <v>6.3261505098731005E-2</v>
+      </c>
+      <c r="P24" s="2">
+        <v>6.3305876519359303E-2</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>6.3961629330528305E-2</v>
+      </c>
+      <c r="R24" s="2">
+        <v>6.3922227191752695E-2</v>
+      </c>
+      <c r="S24" s="2">
+        <v>6.5837958928438203E-2</v>
+      </c>
+      <c r="T24" s="2">
+        <v>6.50854292289232E-2</v>
+      </c>
+      <c r="U24" s="2">
+        <v>6.4574971525459102E-2</v>
+      </c>
+      <c r="V24" s="2">
+        <v>6.4087747692487304E-2</v>
+      </c>
+      <c r="W24" s="5">
+        <v>6.3799946353162204E-2</v>
+      </c>
+      <c r="X24" s="18"/>
     </row>
-    <row r="24" spans="1:16">
-      <c r="A24" s="9" t="s">
+    <row r="25" spans="1:24">
+      <c r="A25" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B25" s="4">
         <v>1.6374929250922501</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C25" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D25" s="4">
         <v>1.70153745105816</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E25" s="4">
         <v>1.6997118491957399</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F25" s="4">
         <v>1.7020967873211601</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G25" s="4">
         <v>1.7008757555040399</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H25" s="4">
         <v>1.70058380671728</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I25" s="4">
         <v>1.6940427706627099</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J25" s="4">
         <v>1.69185950453506</v>
       </c>
-      <c r="K24" s="4">
+      <c r="K25" s="4">
         <v>1.68959747165218</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L25" s="4">
         <v>1.68115796831027</v>
       </c>
-      <c r="M24" s="4">
-        <v>1.6728732103463599</v>
-      </c>
-      <c r="N24" s="4">
-        <v>1.69043947462133</v>
-      </c>
-      <c r="O24" s="4"/>
-      <c r="P24" s="7">
-        <v>1.65869173858881</v>
+      <c r="M25" s="4">
+        <v>1.6790710420066299</v>
+      </c>
+      <c r="N25" s="4">
+        <v>1.68363145391483</v>
+      </c>
+      <c r="O25" s="4">
+        <v>1.6868542874767201</v>
+      </c>
+      <c r="P25" s="4">
+        <v>1.68614781011117</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>1.6760418296573101</v>
+      </c>
+      <c r="R25" s="4">
+        <v>1.67663938831909</v>
+      </c>
+      <c r="S25" s="4">
+        <v>1.6480686744981099</v>
+      </c>
+      <c r="T25" s="4">
+        <v>1.65907725819249</v>
+      </c>
+      <c r="U25" s="4">
+        <v>1.6666597783380299</v>
+      </c>
+      <c r="V25" s="4">
+        <v>1.67397959128549</v>
+      </c>
+      <c r="W25" s="7">
+        <v>1.67834183682618</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
-      <c r="B25" s="2"/>
+    <row r="26" spans="1:24">
+      <c r="B26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>